<commit_message>
read me 1차 추가
</commit_message>
<xml_diff>
--- a/앱스토어 요구사항 명세서(ERD,테이블명세등).xlsx
+++ b/앱스토어 요구사항 명세서(ERD,테이블명세등).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.82\305_공유\3차_프로젝트(웹사이트개발)\1팀_프로젝트방\산출물(회의록,요구사항정의서, 요구사항명세서, 발표PPT)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LJJ\Desktop\이종운 취업\앱스토어 포트폴리오 가공\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF0EDFD-8130-4F93-ABA5-D8C8976EA5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18420" windowHeight="11580" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시나리오" sheetId="7" r:id="rId1"/>
@@ -507,7 +508,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -728,7 +729,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -772,7 +779,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -816,7 +829,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPr id="4" name="그림 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1110,10 +1129,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -1753,11 +1772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1769,10 +1788,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>